<commit_message>
enrichissement de la documentation de l'api
</commit_message>
<xml_diff>
--- a/HydroWit/src/assets/docs/API endpoints.xlsx
+++ b/HydroWit/src/assets/docs/API endpoints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clement_d\code\stageMDE\HydroWit\src\assets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6F2CDD-E2EC-4585-93E1-637A9AAAAB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F45BF5-0E08-458E-8483-C29B8B737B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>Verbe HTTP</t>
   </si>
@@ -57,15 +57,6 @@
     <t>Tableau de données du capteur id:1 de la station id:1 de marégraphe</t>
   </si>
   <si>
-    <t>/field/pluviometrie/stations</t>
-  </si>
-  <si>
-    <t>/field/pluviometrie/stations/id:1/sensors</t>
-  </si>
-  <si>
-    <t>/field/pluviometrie/stations/id:1/sensors/id:1/data</t>
-  </si>
-  <si>
     <t>/field/telemesures/stations</t>
   </si>
   <si>
@@ -75,21 +66,12 @@
     <t>/field/telemesures/stations/id:1/sensors/id:1/data</t>
   </si>
   <si>
-    <t>Liste toutes les stations pluviometrie</t>
-  </si>
-  <si>
     <t>Liste toutes les stations télémesures</t>
   </si>
   <si>
-    <t>Liste tout les capteurs de la station id:1 de pluviometrie</t>
-  </si>
-  <si>
     <t>Liste tout les capteurs de la station id:1 de télémesures</t>
   </si>
   <si>
-    <t>Tableau de données du capteur id:1 de la station id:1 de pluviométrie</t>
-  </si>
-  <si>
     <t>Tableau de données du capteur id:1 de la station id:1 de télémesures</t>
   </si>
   <si>
@@ -114,12 +96,6 @@
     <t>Liste tout les capteurs de la station id:1 de marégraphe</t>
   </si>
   <si>
-    <t>/field/pluviometrie/stations/id:1/data</t>
-  </si>
-  <si>
-    <t>Tableau de données de la station id:1 de pluviomerie</t>
-  </si>
-  <si>
     <t>/field/telemesures/stations/id:1/data</t>
   </si>
   <si>
@@ -175,6 +151,78 @@
   </si>
   <si>
     <t>Supprimer l'intervention id:1</t>
+  </si>
+  <si>
+    <t>Valeurs de retour</t>
+  </si>
+  <si>
+    <t>Nom de chaque station</t>
+  </si>
+  <si>
+    <t>Nom de chaque capteur</t>
+  </si>
+  <si>
+    <t>Nom de chaque station marégraphe</t>
+  </si>
+  <si>
+    <t>Nom de chaque station télémesures</t>
+  </si>
+  <si>
+    <t>Nom de chaque station pluviométrie</t>
+  </si>
+  <si>
+    <t>Nom de chaque capteur de la station marégraphe</t>
+  </si>
+  <si>
+    <t>Nom de chaque capteur de la station pluviométrie</t>
+  </si>
+  <si>
+    <t>Nom de chaque capteur de la station télémesures</t>
+  </si>
+  <si>
+    <t>Nom de la station, nom du capteur, date de la mesure, heure de la mesure, donnée de la mesure</t>
+  </si>
+  <si>
+    <t>Nom de la station, nom des capteurs, date de la mesure, heure de la mesure, données de la mesure</t>
+  </si>
+  <si>
+    <t>Nom de la station, noms des capteurs, date de la mesure, heure de la mesure, données de la mesure</t>
+  </si>
+  <si>
+    <t>Numéro et titre de chaque intervention</t>
+  </si>
+  <si>
+    <t>Numéro, titre, date, heure, contenu de l'intervention</t>
+  </si>
+  <si>
+    <t>Nom, prénom, rang de chaque utilisateur</t>
+  </si>
+  <si>
+    <t>Nom, prénom, rang, nombre d'interventions créées de l'utilisateur</t>
+  </si>
+  <si>
+    <t>/field/meteorologie/stations</t>
+  </si>
+  <si>
+    <t>/field/meteorologie/stations/id:1/sensors</t>
+  </si>
+  <si>
+    <t>/field/meteorologie/stations/id:1/data</t>
+  </si>
+  <si>
+    <t>/field/meteorologie/stations/id:1/sensors/id:1/data</t>
+  </si>
+  <si>
+    <t>Liste toutes les stations meteorologie</t>
+  </si>
+  <si>
+    <t>Liste tout les capteurs de la station id:1 de meteorologie</t>
+  </si>
+  <si>
+    <t>Tableau de données de la station id:1 de meteorologie</t>
+  </si>
+  <si>
+    <t>Tableau de données du capteur id:1 de la station id:1 de meteorologie</t>
   </si>
 </sst>
 </file>
@@ -206,7 +254,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -331,11 +379,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -346,7 +446,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -360,17 +459,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,315 +787,380 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:D32"/>
+  <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="62.140625" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="14"/>
-    </row>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="26"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="E20" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="26"/>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="23"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="C24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="2:5" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C26" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="D26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="C27" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="23"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
     </row>
   </sheetData>
@@ -971,6 +1168,6 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="97" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MAJ README, ajout d'un endpoint de l'API.
</commit_message>
<xml_diff>
--- a/HydroWit/src/assets/docs/API endpoints.xlsx
+++ b/HydroWit/src/assets/docs/API endpoints.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clement_d\code\stageMDE\HydroWit\src\assets\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Administratif\Travail\Formation AFPA DWWM\Workspace\Code\stageMDE\HydroWit\src\assets\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A6ACA5-7770-408F-9B69-8A52F2A1DBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>Verbe HTTP</t>
   </si>
@@ -181,12 +180,18 @@
   </si>
   <si>
     <t>Tableau de données de tous les capteurs id:1</t>
+  </si>
+  <si>
+    <t>/healthcheck</t>
+  </si>
+  <si>
+    <t>Vérifie l'état de l'API</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -395,12 +400,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -420,8 +419,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,14 +716,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N33"/>
+  <dimension ref="B1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,36 +731,36 @@
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="47.140625" customWidth="1"/>
     <col min="4" max="4" width="62.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="25" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
@@ -755,560 +769,581 @@
       <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+    </row>
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="25"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-    </row>
-    <row r="6" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="14" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+    </row>
+    <row r="7" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D7" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="22"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="E7" s="26"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="24" t="s">
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-    </row>
-    <row r="9" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="23" t="s">
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+    </row>
+    <row r="10" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-    </row>
-    <row r="10" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="14" t="s">
+      <c r="E10" s="26"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+    </row>
+    <row r="11" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="E11" s="26"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="24" t="s">
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-    </row>
-    <row r="13" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="23" t="s">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-    </row>
-    <row r="14" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="14" t="s">
+      <c r="E14" s="26"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+    </row>
+    <row r="15" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D15" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-    </row>
-    <row r="15" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="E15" s="26"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
+    </row>
+    <row r="16" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-    </row>
-    <row r="17" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="23" t="s">
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+    </row>
+    <row r="18" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-    </row>
-    <row r="18" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="E18" s="26"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+    </row>
+    <row r="19" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="E19" s="26"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
+        <v>40</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C23" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-    </row>
-    <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="7" t="s">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+    </row>
+    <row r="24" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C26" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-    </row>
-    <row r="26" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="23" t="s">
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+    </row>
+    <row r="27" spans="2:14" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D27" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="28"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
+      <c r="E27" s="26"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C28" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-    </row>
-    <row r="28" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="7" t="s">
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+    </row>
+    <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C29" s="1"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C30" s="1"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C31" s="1"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>